<commit_message>
Updated Semi File file
</commit_message>
<xml_diff>
--- a/Financial_Data/MoneyControl/Companies/IT Services & Consulting/3i Infotech Ltd/Pruned_Excel/Final_Parameters/Semi_Final/3i Infotech Ltd_Semi_Final.xlsx
+++ b/Financial_Data/MoneyControl/Companies/IT Services & Consulting/3i Infotech Ltd/Pruned_Excel/Final_Parameters/Semi_Final/3i Infotech Ltd_Semi_Final.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="123">
   <si>
     <t>Balance Sheet of 3i Infotech(in Rs. Cr.)</t>
   </si>
@@ -215,6 +215,12 @@
     <t>Quarterly Results of 3i Infotech(in Rs. Cr.)</t>
   </si>
   <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Quarter</t>
+  </si>
+  <si>
     <t>Net sales/income from operations</t>
   </si>
   <si>
@@ -269,139 +275,64 @@
     <t>Diluted eps.</t>
   </si>
   <si>
-    <t>Sep 13 Q2</t>
-  </si>
-  <si>
-    <t>Dec 13 Q3</t>
-  </si>
-  <si>
-    <t>Mar 14 Q4</t>
-  </si>
-  <si>
-    <t>Jun 14 Q1</t>
-  </si>
-  <si>
-    <t>Sep 14 Q2</t>
-  </si>
-  <si>
-    <t>Dec 14 Q3</t>
-  </si>
-  <si>
-    <t>Mar 15 Q4</t>
-  </si>
-  <si>
-    <t>Jun 15 Q1</t>
-  </si>
-  <si>
-    <t>Sep 15 Q2</t>
-  </si>
-  <si>
-    <t>Dec 15 Q3</t>
-  </si>
-  <si>
-    <t>Mar 16 Q4</t>
-  </si>
-  <si>
-    <t>Jun 16 Q1</t>
-  </si>
-  <si>
-    <t>Sep 16 Q2</t>
-  </si>
-  <si>
-    <t>Dec 16 Q3</t>
-  </si>
-  <si>
-    <t>Mar 17 Q4</t>
-  </si>
-  <si>
-    <t>Jun 17 Q1</t>
-  </si>
-  <si>
-    <t>Sep 17 Q2</t>
-  </si>
-  <si>
-    <t>Dec 17 Q3</t>
-  </si>
-  <si>
-    <t>Mar 18 Q4</t>
-  </si>
-  <si>
-    <t>Jun 18 Q1</t>
-  </si>
-  <si>
-    <t>Sep 18 Q2</t>
-  </si>
-  <si>
-    <t>Dec 18 Q3</t>
-  </si>
-  <si>
-    <t>Mar 19 Q4</t>
-  </si>
-  <si>
-    <t>Jun 19 Q1</t>
-  </si>
-  <si>
-    <t>Sep 19 Q2</t>
-  </si>
-  <si>
-    <t>Dec 19 Q3</t>
-  </si>
-  <si>
-    <t>Mar 20 Q4</t>
-  </si>
-  <si>
-    <t>Jun 20 Q1</t>
-  </si>
-  <si>
-    <t>Sep 20 Q2</t>
-  </si>
-  <si>
-    <t>Dec 20 Q3</t>
-  </si>
-  <si>
-    <t>Mar 21 Q4</t>
-  </si>
-  <si>
-    <t>Jun 21 Q1</t>
-  </si>
-  <si>
-    <t>Sep 21 Q2</t>
-  </si>
-  <si>
-    <t>Dec 21 Q3</t>
-  </si>
-  <si>
-    <t>Mar 22 Q4</t>
-  </si>
-  <si>
-    <t>Jun 22 Q1</t>
-  </si>
-  <si>
-    <t>Sep 22 Q2</t>
-  </si>
-  <si>
-    <t>Dec 22 Q3</t>
-  </si>
-  <si>
-    <t>Mar 23 Q4</t>
-  </si>
-  <si>
-    <t>Jun 23 Q1</t>
-  </si>
-  <si>
-    <t>Sep 23 Q2</t>
-  </si>
-  <si>
-    <t>Dec 23 Q3</t>
-  </si>
-  <si>
-    <t>Mar 24 Q4</t>
-  </si>
-  <si>
-    <t>Jun 24 Q1</t>
-  </si>
-  <si>
-    <t>Sep 24 Q2</t>
+    <t>2013</t>
+  </si>
+  <si>
+    <t>2014</t>
+  </si>
+  <si>
+    <t>2015</t>
+  </si>
+  <si>
+    <t>2016</t>
+  </si>
+  <si>
+    <t>2017</t>
+  </si>
+  <si>
+    <t>2018</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>2020</t>
+  </si>
+  <si>
+    <t>2021</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>2024</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q1</t>
   </si>
   <si>
     <t>Key Financial Ratios of 3i Infotech(in Rs. Cr.)</t>
@@ -3750,13 +3681,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U46"/>
+  <dimension ref="A1:W46"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:23">
       <c r="A1" s="1" t="s">
         <v>64</v>
       </c>
@@ -3773,19 +3704,19 @@
         <v>68</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>72</v>
@@ -3820,64 +3751,70 @@
       <c r="U1" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="V1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
       <c r="A2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B2">
+        <v>85</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D2">
         <v>78.26000000000001</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>78.26000000000001</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>38.63</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>55.44</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>27.47</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>-43.28</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>21.86</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>-21.42</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>74.56</v>
-      </c>
-      <c r="K2">
-        <v>-95.98</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
       </c>
       <c r="M2">
         <v>-95.98</v>
       </c>
       <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>-95.98</v>
+      </c>
+      <c r="P2">
         <v>1.5</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>-97.48</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>-97.48</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>571.9400000000001</v>
-      </c>
-      <c r="R2">
-        <v>-1.79</v>
-      </c>
-      <c r="S2">
-        <v>-1.79</v>
       </c>
       <c r="T2">
         <v>-1.79</v>
@@ -3885,64 +3822,70 @@
       <c r="U2">
         <v>-1.79</v>
       </c>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="V2">
+        <v>-1.79</v>
+      </c>
+      <c r="W2">
+        <v>-1.79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3">
         <v>90.95</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>90.95</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>43.95</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>67.06999999999999</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>30.53</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>-50.6</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>-1.12</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>-51.72</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>87.48999999999999</v>
-      </c>
-      <c r="K3">
-        <v>-139.21</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
       </c>
       <c r="M3">
         <v>-139.21</v>
       </c>
       <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>-139.21</v>
+      </c>
+      <c r="P3">
         <v>0.23</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>-139.44</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>-139.44</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>571.9400000000001</v>
-      </c>
-      <c r="R3">
-        <v>-2.52</v>
-      </c>
-      <c r="S3">
-        <v>-2.52</v>
       </c>
       <c r="T3">
         <v>-2.52</v>
@@ -3950,108 +3893,120 @@
       <c r="U3">
         <v>-2.52</v>
       </c>
-    </row>
-    <row r="4" spans="1:21">
+      <c r="V3">
+        <v>-2.52</v>
+      </c>
+      <c r="W3">
+        <v>-2.52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4">
         <v>79.08</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>79.08</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>41.18</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>57.31</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>27.76</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>-47.17</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>10.78</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>-36.39</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>64.37</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>-100.76</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>-35.85</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>-136.61</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>-15.28</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>-121.33</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>-121.33</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>572.64</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>-1.58</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>-1.58</v>
       </c>
-      <c r="T4">
+      <c r="V4">
         <v>-2.2</v>
       </c>
-      <c r="U4">
+      <c r="W4">
         <v>-2.2</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:23">
       <c r="A5" t="s">
         <v>86</v>
       </c>
-      <c r="B5">
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5">
         <v>93.17</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>93.17</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>43.9</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>58.04</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>41.54</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>-50.31</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>1.39</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>-48.92</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>56.29</v>
-      </c>
-      <c r="K5">
-        <v>-105.21</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
       </c>
       <c r="M5">
         <v>-105.21</v>
@@ -4063,16 +4018,16 @@
         <v>-105.21</v>
       </c>
       <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
         <v>-105.21</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
+        <v>-105.21</v>
+      </c>
+      <c r="S5">
         <v>576.34</v>
-      </c>
-      <c r="R5">
-        <v>-1.92</v>
-      </c>
-      <c r="S5">
-        <v>-1.92</v>
       </c>
       <c r="T5">
         <v>-1.92</v>
@@ -4080,43 +4035,49 @@
       <c r="U5">
         <v>-1.92</v>
       </c>
-    </row>
-    <row r="6" spans="1:21">
+      <c r="V5">
+        <v>-1.92</v>
+      </c>
+      <c r="W5">
+        <v>-1.92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23">
       <c r="A6" t="s">
-        <v>87</v>
-      </c>
-      <c r="B6">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" t="s">
+        <v>101</v>
+      </c>
+      <c r="D6">
         <v>108.29</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>108.29</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>42.54</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>52.49</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>61.74</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>-48.48</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>0.1</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>-48.38</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>52.02</v>
-      </c>
-      <c r="K6">
-        <v>-100.4</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
       </c>
       <c r="M6">
         <v>-100.4</v>
@@ -4128,16 +4089,16 @@
         <v>-100.4</v>
       </c>
       <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
         <v>-100.4</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
+        <v>-100.4</v>
+      </c>
+      <c r="S6">
         <v>580.6799999999999</v>
-      </c>
-      <c r="R6">
-        <v>-1.82</v>
-      </c>
-      <c r="S6">
-        <v>-1.82</v>
       </c>
       <c r="T6">
         <v>-1.82</v>
@@ -4145,173 +4106,191 @@
       <c r="U6">
         <v>-1.82</v>
       </c>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="V6">
+        <v>-1.82</v>
+      </c>
+      <c r="W6">
+        <v>-1.82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B7">
+        <v>86</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7">
         <v>105.8</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>105.8</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>40.21</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>55.05</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>78.29000000000001</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>-67.75</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>0.41</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>-67.34</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>52.03</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>-119.37</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>-329.79</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>-449.16</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>2.02</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>-451.18</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>-451.18</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>586.12</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <v>-2.17</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <v>-2.17</v>
       </c>
-      <c r="T7">
+      <c r="V7">
         <v>-7.84</v>
       </c>
-      <c r="U7">
+      <c r="W7">
         <v>-7.84</v>
       </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8">
+        <v>87</v>
+      </c>
+      <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" t="s">
+        <v>103</v>
+      </c>
+      <c r="D8">
         <v>93.45999999999999</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>93.45999999999999</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>25.21</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>57.31</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>-2.67</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>13.61</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>2.14</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>15.75</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>34.35</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>-18.6</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>-360.82</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>-379.42</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>21.54</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>-400.96</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>-400.96</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>603.75</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>-0.76</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>-0.76</v>
       </c>
-      <c r="T8">
+      <c r="V8">
         <v>-6.84</v>
       </c>
-      <c r="U8">
+      <c r="W8">
         <v>-6.84</v>
       </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9">
+        <v>87</v>
+      </c>
+      <c r="B9" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9">
         <v>81.77</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>81.77</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>38.57</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>51.51</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>46.3</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>-54.61</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>0.49</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>-54.12</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>47.4</v>
-      </c>
-      <c r="K9">
-        <v>-101.52</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
       </c>
       <c r="M9">
         <v>-101.52</v>
@@ -4323,16 +4302,16 @@
         <v>-101.52</v>
       </c>
       <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
         <v>-101.52</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
+        <v>-101.52</v>
+      </c>
+      <c r="S9">
         <v>612.4299999999999</v>
-      </c>
-      <c r="R9">
-        <v>-1.75</v>
-      </c>
-      <c r="S9">
-        <v>-1.75</v>
       </c>
       <c r="T9">
         <v>-1.75</v>
@@ -4340,43 +4319,49 @@
       <c r="U9">
         <v>-1.75</v>
       </c>
-    </row>
-    <row r="10" spans="1:21">
+      <c r="V9">
+        <v>-1.75</v>
+      </c>
+      <c r="W9">
+        <v>-1.75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B10">
+        <v>87</v>
+      </c>
+      <c r="B10" t="s">
+        <v>97</v>
+      </c>
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10">
         <v>84.08</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>84.08</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>32.35</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>51.9</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>68.69</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>-68.86</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>0.74</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>-68.12</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>43.79</v>
-      </c>
-      <c r="K10">
-        <v>-111.91</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
       </c>
       <c r="M10">
         <v>-111.91</v>
@@ -4388,16 +4373,16 @@
         <v>-111.91</v>
       </c>
       <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
         <v>-111.91</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
+        <v>-111.91</v>
+      </c>
+      <c r="S10">
         <v>612.52</v>
-      </c>
-      <c r="R10">
-        <v>-1.91</v>
-      </c>
-      <c r="S10">
-        <v>-1.91</v>
       </c>
       <c r="T10">
         <v>-1.91</v>
@@ -4405,43 +4390,49 @@
       <c r="U10">
         <v>-1.91</v>
       </c>
-    </row>
-    <row r="11" spans="1:21">
+      <c r="V10">
+        <v>-1.91</v>
+      </c>
+      <c r="W10">
+        <v>-1.91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B11">
+        <v>87</v>
+      </c>
+      <c r="B11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11">
         <v>79.54000000000001</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>79.54000000000001</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>22.27</v>
       </c>
-      <c r="E11">
+      <c r="G11">
         <v>52.22</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>23.61</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>-18.56</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>43.2</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>24.64</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>42.29</v>
-      </c>
-      <c r="K11">
-        <v>-17.65</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
       </c>
       <c r="M11">
         <v>-17.65</v>
@@ -4453,16 +4444,16 @@
         <v>-17.65</v>
       </c>
       <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
         <v>-17.65</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
+        <v>-17.65</v>
+      </c>
+      <c r="S11">
         <v>636.1900000000001</v>
-      </c>
-      <c r="R11">
-        <v>-0.36</v>
-      </c>
-      <c r="S11">
-        <v>-0.36</v>
       </c>
       <c r="T11">
         <v>-0.36</v>
@@ -4470,64 +4461,70 @@
       <c r="U11">
         <v>-0.36</v>
       </c>
-    </row>
-    <row r="12" spans="1:21">
+      <c r="V11">
+        <v>-0.36</v>
+      </c>
+      <c r="W11">
+        <v>-0.36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12">
+        <v>88</v>
+      </c>
+      <c r="B12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12">
         <v>84.84999999999999</v>
       </c>
-      <c r="C12">
+      <c r="E12">
         <v>84.84999999999999</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>17.56</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>55</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>15.03</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>-2.74</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>2.02</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>-0.72</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>6.68</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>-7.4</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>-698.03</v>
       </c>
-      <c r="M12">
+      <c r="O12">
         <v>-705.4299999999999</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <v>127.15</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>-832.58</v>
       </c>
-      <c r="P12">
+      <c r="R12">
         <v>-832.58</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <v>640.8</v>
-      </c>
-      <c r="R12">
-        <v>-2.1</v>
-      </c>
-      <c r="S12">
-        <v>-2.1</v>
       </c>
       <c r="T12">
         <v>-2.1</v>
@@ -4535,43 +4532,49 @@
       <c r="U12">
         <v>-2.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:21">
+      <c r="V12">
+        <v>-2.1</v>
+      </c>
+      <c r="W12">
+        <v>-2.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B13">
+        <v>88</v>
+      </c>
+      <c r="B13" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" t="s">
+        <v>104</v>
+      </c>
+      <c r="D13">
         <v>81.33</v>
       </c>
-      <c r="C13">
+      <c r="E13">
         <v>81.33</v>
       </c>
-      <c r="D13">
+      <c r="F13">
         <v>39.75</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <v>2.29</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <v>17.57</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>21.72</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>16.7</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>38.42</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>22.91</v>
-      </c>
-      <c r="K13">
-        <v>15.51</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
       </c>
       <c r="M13">
         <v>15.51</v>
@@ -4583,16 +4586,16 @@
         <v>15.51</v>
       </c>
       <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
         <v>15.51</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
+        <v>15.51</v>
+      </c>
+      <c r="S13">
         <v>640.8</v>
-      </c>
-      <c r="R13">
-        <v>0.24</v>
-      </c>
-      <c r="S13">
-        <v>0.24</v>
       </c>
       <c r="T13">
         <v>0.24</v>
@@ -4600,64 +4603,70 @@
       <c r="U13">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="14" spans="1:21">
+      <c r="V13">
+        <v>0.24</v>
+      </c>
+      <c r="W13">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>95</v>
-      </c>
-      <c r="B14">
+        <v>88</v>
+      </c>
+      <c r="B14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" t="s">
+        <v>101</v>
+      </c>
+      <c r="D14">
         <v>55.93</v>
       </c>
-      <c r="C14">
+      <c r="E14">
         <v>55.93</v>
       </c>
-      <c r="D14">
+      <c r="F14">
         <v>24.61</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>1.54</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <v>9.210000000000001</v>
       </c>
-      <c r="G14">
+      <c r="I14">
         <v>20.57</v>
       </c>
-      <c r="H14">
+      <c r="J14">
         <v>15.05</v>
       </c>
-      <c r="I14">
+      <c r="K14">
         <v>35.62</v>
       </c>
-      <c r="J14">
+      <c r="L14">
         <v>21.18</v>
-      </c>
-      <c r="K14">
-        <v>14.44</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
       </c>
       <c r="M14">
         <v>14.44</v>
       </c>
       <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>14.44</v>
+      </c>
+      <c r="P14">
         <v>0.19</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>14.25</v>
       </c>
-      <c r="P14">
+      <c r="R14">
         <v>14.25</v>
       </c>
-      <c r="Q14">
+      <c r="S14">
         <v>898.88</v>
-      </c>
-      <c r="R14">
-        <v>0.3</v>
-      </c>
-      <c r="S14">
-        <v>0.15</v>
       </c>
       <c r="T14">
         <v>0.3</v>
@@ -4665,43 +4674,49 @@
       <c r="U14">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="15" spans="1:21">
+      <c r="V14">
+        <v>0.3</v>
+      </c>
+      <c r="W14">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23">
       <c r="A15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15">
+        <v>88</v>
+      </c>
+      <c r="B15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15">
         <v>64.56999999999999</v>
       </c>
-      <c r="C15">
+      <c r="E15">
         <v>64.56999999999999</v>
       </c>
-      <c r="D15">
+      <c r="F15">
         <v>6.49</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <v>1.76</v>
       </c>
-      <c r="F15">
+      <c r="H15">
         <v>21.2</v>
       </c>
-      <c r="G15">
+      <c r="I15">
         <v>35.12</v>
       </c>
-      <c r="H15">
+      <c r="J15">
         <v>44.05</v>
       </c>
-      <c r="I15">
+      <c r="K15">
         <v>79.17</v>
       </c>
-      <c r="J15">
+      <c r="L15">
         <v>22.38</v>
-      </c>
-      <c r="K15">
-        <v>56.79</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
       </c>
       <c r="M15">
         <v>56.79</v>
@@ -4713,16 +4728,16 @@
         <v>56.79</v>
       </c>
       <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
         <v>56.79</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
+        <v>56.79</v>
+      </c>
+      <c r="S15">
         <v>1047.45</v>
-      </c>
-      <c r="R15">
-        <v>0.52</v>
-      </c>
-      <c r="S15">
-        <v>0.52</v>
       </c>
       <c r="T15">
         <v>0.52</v>
@@ -4730,64 +4745,70 @@
       <c r="U15">
         <v>0.52</v>
       </c>
-    </row>
-    <row r="16" spans="1:21">
+      <c r="V15">
+        <v>0.52</v>
+      </c>
+      <c r="W15">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23">
       <c r="A16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B16">
+        <v>89</v>
+      </c>
+      <c r="B16" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16">
         <v>66.98999999999999</v>
       </c>
-      <c r="C16">
+      <c r="E16">
         <v>66.98999999999999</v>
       </c>
-      <c r="D16">
+      <c r="F16">
         <v>19.96</v>
       </c>
-      <c r="E16">
+      <c r="G16">
         <v>1.71</v>
       </c>
-      <c r="F16">
+      <c r="H16">
         <v>11.89</v>
       </c>
-      <c r="G16">
+      <c r="I16">
         <v>33.43</v>
       </c>
-      <c r="H16">
+      <c r="J16">
         <v>17.32</v>
       </c>
-      <c r="I16">
+      <c r="K16">
         <v>50.75</v>
       </c>
-      <c r="J16">
+      <c r="L16">
         <v>20.8</v>
       </c>
-      <c r="K16">
+      <c r="M16">
         <v>29.95</v>
       </c>
-      <c r="L16">
+      <c r="N16">
         <v>-25.6</v>
       </c>
-      <c r="M16">
+      <c r="O16">
         <v>4.35</v>
       </c>
-      <c r="N16">
+      <c r="P16">
         <v>-1.37</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>5.72</v>
       </c>
-      <c r="P16">
+      <c r="R16">
         <v>5.72</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <v>1183.65</v>
-      </c>
-      <c r="R16">
-        <v>0.05</v>
-      </c>
-      <c r="S16">
-        <v>0.05</v>
       </c>
       <c r="T16">
         <v>0.05</v>
@@ -4795,64 +4816,70 @@
       <c r="U16">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="17" spans="1:21">
+      <c r="V16">
+        <v>0.05</v>
+      </c>
+      <c r="W16">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
       <c r="A17" t="s">
-        <v>98</v>
-      </c>
-      <c r="B17">
+        <v>89</v>
+      </c>
+      <c r="B17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C17" t="s">
+        <v>104</v>
+      </c>
+      <c r="D17">
         <v>55.38</v>
       </c>
-      <c r="C17">
+      <c r="E17">
         <v>55.38</v>
       </c>
-      <c r="D17">
+      <c r="F17">
         <v>16.68</v>
       </c>
-      <c r="E17">
+      <c r="G17">
         <v>1.78</v>
       </c>
-      <c r="F17">
+      <c r="H17">
         <v>15.53</v>
       </c>
-      <c r="G17">
+      <c r="I17">
         <v>21.39</v>
       </c>
-      <c r="H17">
+      <c r="J17">
         <v>9.380000000000001</v>
       </c>
-      <c r="I17">
+      <c r="K17">
         <v>30.77</v>
       </c>
-      <c r="J17">
+      <c r="L17">
         <v>12.01</v>
       </c>
-      <c r="K17">
+      <c r="M17">
         <v>18.76</v>
       </c>
-      <c r="L17">
+      <c r="N17">
         <v>-3.05</v>
-      </c>
-      <c r="M17">
-        <v>15.71</v>
-      </c>
-      <c r="N17">
-        <v>0</v>
       </c>
       <c r="O17">
         <v>15.71</v>
       </c>
       <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>15.71</v>
+      </c>
+      <c r="R17">
         <v>17.7</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <v>1286</v>
-      </c>
-      <c r="R17">
-        <v>0.14</v>
-      </c>
-      <c r="S17">
-        <v>0.14</v>
       </c>
       <c r="T17">
         <v>0.14</v>
@@ -4860,64 +4887,70 @@
       <c r="U17">
         <v>0.14</v>
       </c>
-    </row>
-    <row r="18" spans="1:21">
+      <c r="V17">
+        <v>0.14</v>
+      </c>
+      <c r="W17">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
       <c r="A18" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18">
+        <v>89</v>
+      </c>
+      <c r="B18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18">
         <v>57.72</v>
       </c>
-      <c r="C18">
+      <c r="E18">
         <v>57.72</v>
       </c>
-      <c r="D18">
+      <c r="F18">
         <v>22.5</v>
       </c>
-      <c r="E18">
+      <c r="G18">
         <v>2.05</v>
       </c>
-      <c r="F18">
+      <c r="H18">
         <v>162.13</v>
       </c>
-      <c r="G18">
+      <c r="I18">
         <v>-128.96</v>
       </c>
-      <c r="H18">
+      <c r="J18">
         <v>2.96</v>
       </c>
-      <c r="I18">
+      <c r="K18">
         <v>-126</v>
       </c>
-      <c r="J18">
+      <c r="L18">
         <v>12.21</v>
       </c>
-      <c r="K18">
+      <c r="M18">
         <v>-138.21</v>
       </c>
-      <c r="L18">
+      <c r="N18">
         <v>12.22</v>
-      </c>
-      <c r="M18">
-        <v>-125.99</v>
-      </c>
-      <c r="N18">
-        <v>0</v>
       </c>
       <c r="O18">
         <v>-125.99</v>
       </c>
       <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>-125.99</v>
+      </c>
+      <c r="R18">
         <v>-130.09</v>
       </c>
-      <c r="Q18">
+      <c r="S18">
         <v>1333.09</v>
-      </c>
-      <c r="R18">
-        <v>-0.99</v>
-      </c>
-      <c r="S18">
-        <v>-0.99</v>
       </c>
       <c r="T18">
         <v>-0.99</v>
@@ -4925,64 +4958,70 @@
       <c r="U18">
         <v>-0.99</v>
       </c>
-    </row>
-    <row r="19" spans="1:21">
+      <c r="V18">
+        <v>-0.99</v>
+      </c>
+      <c r="W18">
+        <v>-0.99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23">
       <c r="A19" t="s">
-        <v>100</v>
-      </c>
-      <c r="B19">
+        <v>89</v>
+      </c>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D19">
         <v>58.12</v>
       </c>
-      <c r="C19">
+      <c r="E19">
         <v>58.12</v>
       </c>
-      <c r="D19">
+      <c r="F19">
         <v>14.68</v>
       </c>
-      <c r="E19">
+      <c r="G19">
         <v>1.7</v>
       </c>
-      <c r="F19">
+      <c r="H19">
         <v>17.27</v>
       </c>
-      <c r="G19">
+      <c r="I19">
         <v>24.47</v>
       </c>
-      <c r="H19">
+      <c r="J19">
         <v>8.25</v>
       </c>
-      <c r="I19">
+      <c r="K19">
         <v>32.72</v>
       </c>
-      <c r="J19">
+      <c r="L19">
         <v>12.37</v>
       </c>
-      <c r="K19">
+      <c r="M19">
         <v>20.35</v>
       </c>
-      <c r="L19">
+      <c r="N19">
         <v>-18.4</v>
-      </c>
-      <c r="M19">
-        <v>1.95</v>
-      </c>
-      <c r="N19">
-        <v>0</v>
       </c>
       <c r="O19">
         <v>1.95</v>
       </c>
       <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>1.95</v>
+      </c>
+      <c r="R19">
         <v>-2.1</v>
       </c>
-      <c r="Q19">
+      <c r="S19">
         <v>1334.15</v>
-      </c>
-      <c r="R19">
-        <v>-0.02</v>
-      </c>
-      <c r="S19">
-        <v>-0.02</v>
       </c>
       <c r="T19">
         <v>-0.02</v>
@@ -4990,64 +5029,70 @@
       <c r="U19">
         <v>-0.02</v>
       </c>
-    </row>
-    <row r="20" spans="1:21">
+      <c r="V19">
+        <v>-0.02</v>
+      </c>
+      <c r="W19">
+        <v>-0.02</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23">
       <c r="A20" t="s">
-        <v>101</v>
-      </c>
-      <c r="B20">
+        <v>90</v>
+      </c>
+      <c r="B20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C20" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20">
         <v>66.29000000000001</v>
       </c>
-      <c r="C20">
+      <c r="E20">
         <v>66.29000000000001</v>
       </c>
-      <c r="D20">
+      <c r="F20">
         <v>24.08</v>
       </c>
-      <c r="E20">
+      <c r="G20">
         <v>1.63</v>
       </c>
-      <c r="F20">
+      <c r="H20">
         <v>18.62</v>
       </c>
-      <c r="G20">
+      <c r="I20">
         <v>21.96</v>
       </c>
-      <c r="H20">
+      <c r="J20">
         <v>4.33</v>
       </c>
-      <c r="I20">
+      <c r="K20">
         <v>26.29</v>
       </c>
-      <c r="J20">
+      <c r="L20">
         <v>11.44</v>
       </c>
-      <c r="K20">
+      <c r="M20">
         <v>14.85</v>
       </c>
-      <c r="L20">
+      <c r="N20">
         <v>17.35</v>
-      </c>
-      <c r="M20">
-        <v>32.2</v>
-      </c>
-      <c r="N20">
-        <v>0</v>
       </c>
       <c r="O20">
         <v>32.2</v>
       </c>
       <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>32.2</v>
+      </c>
+      <c r="R20">
         <v>27.75</v>
       </c>
-      <c r="Q20">
+      <c r="S20">
         <v>1615.36</v>
-      </c>
-      <c r="R20">
-        <v>0.17</v>
-      </c>
-      <c r="S20">
-        <v>0.17</v>
       </c>
       <c r="T20">
         <v>0.17</v>
@@ -5055,64 +5100,70 @@
       <c r="U20">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="21" spans="1:21">
+      <c r="V20">
+        <v>0.17</v>
+      </c>
+      <c r="W20">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23">
       <c r="A21" t="s">
-        <v>102</v>
-      </c>
-      <c r="B21">
+        <v>90</v>
+      </c>
+      <c r="B21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21">
         <v>58.7</v>
       </c>
-      <c r="C21">
+      <c r="E21">
         <v>58.7</v>
       </c>
-      <c r="D21">
+      <c r="F21">
         <v>28.2</v>
       </c>
-      <c r="E21">
+      <c r="G21">
         <v>1.66</v>
       </c>
-      <c r="F21">
+      <c r="H21">
         <v>22.54</v>
       </c>
-      <c r="G21">
+      <c r="I21">
         <v>6.3</v>
       </c>
-      <c r="H21">
+      <c r="J21">
         <v>8.68</v>
       </c>
-      <c r="I21">
+      <c r="K21">
         <v>14.98</v>
       </c>
-      <c r="J21">
+      <c r="L21">
         <v>11.22</v>
       </c>
-      <c r="K21">
+      <c r="M21">
         <v>3.76</v>
       </c>
-      <c r="L21">
+      <c r="N21">
         <v>40.47</v>
-      </c>
-      <c r="M21">
-        <v>44.23</v>
-      </c>
-      <c r="N21">
-        <v>0</v>
       </c>
       <c r="O21">
         <v>44.23</v>
       </c>
       <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>44.23</v>
+      </c>
+      <c r="R21">
         <v>39.54</v>
       </c>
-      <c r="Q21">
+      <c r="S21">
         <v>1615.55</v>
-      </c>
-      <c r="R21">
-        <v>0.24</v>
-      </c>
-      <c r="S21">
-        <v>0.24</v>
       </c>
       <c r="T21">
         <v>0.24</v>
@@ -5120,64 +5171,70 @@
       <c r="U21">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="22" spans="1:21">
+      <c r="V21">
+        <v>0.24</v>
+      </c>
+      <c r="W21">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
       <c r="A22" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22">
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22">
         <v>75.67</v>
       </c>
-      <c r="C22">
+      <c r="E22">
         <v>75.67</v>
       </c>
-      <c r="D22">
+      <c r="F22">
         <v>17.85</v>
       </c>
-      <c r="E22">
+      <c r="G22">
         <v>1.68</v>
       </c>
-      <c r="F22">
+      <c r="H22">
         <v>17.44</v>
       </c>
-      <c r="G22">
+      <c r="I22">
         <v>38.7</v>
       </c>
-      <c r="H22">
+      <c r="J22">
         <v>2.51</v>
       </c>
-      <c r="I22">
+      <c r="K22">
         <v>41.21</v>
       </c>
-      <c r="J22">
+      <c r="L22">
         <v>10.75</v>
       </c>
-      <c r="K22">
+      <c r="M22">
         <v>30.46</v>
       </c>
-      <c r="L22">
+      <c r="N22">
         <v>52.69</v>
-      </c>
-      <c r="M22">
-        <v>83.15000000000001</v>
-      </c>
-      <c r="N22">
-        <v>0</v>
       </c>
       <c r="O22">
         <v>83.15000000000001</v>
       </c>
       <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>83.15000000000001</v>
+      </c>
+      <c r="R22">
         <v>78.61</v>
       </c>
-      <c r="Q22">
+      <c r="S22">
         <v>1615.91</v>
-      </c>
-      <c r="R22">
-        <v>0.49</v>
-      </c>
-      <c r="S22">
-        <v>0.49</v>
       </c>
       <c r="T22">
         <v>0.49</v>
@@ -5185,64 +5242,70 @@
       <c r="U22">
         <v>0.49</v>
       </c>
-    </row>
-    <row r="23" spans="1:21">
+      <c r="V22">
+        <v>0.49</v>
+      </c>
+      <c r="W22">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23">
       <c r="A23" t="s">
-        <v>104</v>
-      </c>
-      <c r="B23">
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D23">
         <v>74.27</v>
       </c>
-      <c r="C23">
+      <c r="E23">
         <v>74.27</v>
       </c>
-      <c r="D23">
+      <c r="F23">
         <v>21.67</v>
       </c>
-      <c r="E23">
+      <c r="G23">
         <v>1.7</v>
       </c>
-      <c r="F23">
+      <c r="H23">
         <v>19.09</v>
       </c>
-      <c r="G23">
+      <c r="I23">
         <v>31.81</v>
       </c>
-      <c r="H23">
+      <c r="J23">
         <v>131.56</v>
       </c>
-      <c r="I23">
+      <c r="K23">
         <v>163.37</v>
       </c>
-      <c r="J23">
+      <c r="L23">
         <v>10.87</v>
       </c>
-      <c r="K23">
+      <c r="M23">
         <v>152.5</v>
       </c>
-      <c r="L23">
+      <c r="N23">
         <v>-37.76</v>
-      </c>
-      <c r="M23">
-        <v>114.74</v>
-      </c>
-      <c r="N23">
-        <v>0</v>
       </c>
       <c r="O23">
         <v>114.74</v>
       </c>
       <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>114.74</v>
+      </c>
+      <c r="R23">
         <v>110.25</v>
       </c>
-      <c r="Q23">
+      <c r="S23">
         <v>1616.64</v>
-      </c>
-      <c r="R23">
-        <v>0.68</v>
-      </c>
-      <c r="S23">
-        <v>0.68</v>
       </c>
       <c r="T23">
         <v>0.68</v>
@@ -5250,64 +5313,70 @@
       <c r="U23">
         <v>0.68</v>
       </c>
-    </row>
-    <row r="24" spans="1:21">
+      <c r="V23">
+        <v>0.68</v>
+      </c>
+      <c r="W23">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
       <c r="A24" t="s">
-        <v>105</v>
-      </c>
-      <c r="B24">
+        <v>91</v>
+      </c>
+      <c r="B24" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" t="s">
+        <v>103</v>
+      </c>
+      <c r="D24">
         <v>75.28</v>
       </c>
-      <c r="C24">
+      <c r="E24">
         <v>75.28</v>
       </c>
-      <c r="D24">
+      <c r="F24">
         <v>20.9</v>
       </c>
-      <c r="E24">
+      <c r="G24">
         <v>1.78</v>
       </c>
-      <c r="F24">
+      <c r="H24">
         <v>19.52</v>
       </c>
-      <c r="G24">
+      <c r="I24">
         <v>33.08</v>
       </c>
-      <c r="H24">
+      <c r="J24">
         <v>7.02</v>
       </c>
-      <c r="I24">
+      <c r="K24">
         <v>40.1</v>
       </c>
-      <c r="J24">
+      <c r="L24">
         <v>9.33</v>
       </c>
-      <c r="K24">
+      <c r="M24">
         <v>30.77</v>
       </c>
-      <c r="L24">
+      <c r="N24">
         <v>-3.72</v>
-      </c>
-      <c r="M24">
-        <v>27.05</v>
-      </c>
-      <c r="N24">
-        <v>0</v>
       </c>
       <c r="O24">
         <v>27.05</v>
       </c>
       <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>27.05</v>
+      </c>
+      <c r="R24">
         <v>22.5</v>
       </c>
-      <c r="Q24">
+      <c r="S24">
         <v>1616.64</v>
-      </c>
-      <c r="R24">
-        <v>0.14</v>
-      </c>
-      <c r="S24">
-        <v>0.14</v>
       </c>
       <c r="T24">
         <v>0.14</v>
@@ -5315,64 +5384,70 @@
       <c r="U24">
         <v>0.14</v>
       </c>
-    </row>
-    <row r="25" spans="1:21">
+      <c r="V24">
+        <v>0.14</v>
+      </c>
+      <c r="W24">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
       <c r="A25" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25">
+        <v>91</v>
+      </c>
+      <c r="B25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" t="s">
+        <v>104</v>
+      </c>
+      <c r="D25">
         <v>74.20999999999999</v>
       </c>
-      <c r="C25">
+      <c r="E25">
         <v>74.20999999999999</v>
       </c>
-      <c r="D25">
+      <c r="F25">
         <v>35</v>
       </c>
-      <c r="E25">
+      <c r="G25">
         <v>3.89</v>
       </c>
-      <c r="F25">
+      <c r="H25">
         <v>17.87</v>
       </c>
-      <c r="G25">
+      <c r="I25">
         <v>17.45</v>
       </c>
-      <c r="H25">
+      <c r="J25">
         <v>3.18</v>
       </c>
-      <c r="I25">
+      <c r="K25">
         <v>20.63</v>
       </c>
-      <c r="J25">
+      <c r="L25">
         <v>11.43</v>
       </c>
-      <c r="K25">
+      <c r="M25">
         <v>9.199999999999999</v>
       </c>
-      <c r="L25">
+      <c r="N25">
         <v>-5.85</v>
-      </c>
-      <c r="M25">
-        <v>3.35</v>
-      </c>
-      <c r="N25">
-        <v>0</v>
       </c>
       <c r="O25">
         <v>3.35</v>
       </c>
       <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>3.35</v>
+      </c>
+      <c r="R25">
         <v>-2.03</v>
       </c>
-      <c r="Q25">
+      <c r="S25">
         <v>1616.64</v>
-      </c>
-      <c r="R25">
-        <v>-0.01</v>
-      </c>
-      <c r="S25">
-        <v>-0.01</v>
       </c>
       <c r="T25">
         <v>-0.01</v>
@@ -5380,64 +5455,70 @@
       <c r="U25">
         <v>-0.01</v>
       </c>
-    </row>
-    <row r="26" spans="1:21">
+      <c r="V25">
+        <v>-0.01</v>
+      </c>
+      <c r="W25">
+        <v>-0.01</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
       <c r="A26" t="s">
-        <v>107</v>
-      </c>
-      <c r="B26">
+        <v>91</v>
+      </c>
+      <c r="B26" t="s">
+        <v>97</v>
+      </c>
+      <c r="C26" t="s">
+        <v>101</v>
+      </c>
+      <c r="D26">
         <v>80.98</v>
       </c>
-      <c r="C26">
+      <c r="E26">
         <v>80.98</v>
       </c>
-      <c r="D26">
+      <c r="F26">
         <v>30.29</v>
       </c>
-      <c r="E26">
+      <c r="G26">
         <v>4.06</v>
       </c>
-      <c r="F26">
+      <c r="H26">
         <v>19.96</v>
       </c>
-      <c r="G26">
+      <c r="I26">
         <v>26.67</v>
       </c>
-      <c r="H26">
+      <c r="J26">
         <v>2.23</v>
       </c>
-      <c r="I26">
+      <c r="K26">
         <v>28.9</v>
       </c>
-      <c r="J26">
+      <c r="L26">
         <v>11.18</v>
       </c>
-      <c r="K26">
+      <c r="M26">
         <v>17.72</v>
       </c>
-      <c r="L26">
+      <c r="N26">
         <v>15.75</v>
-      </c>
-      <c r="M26">
-        <v>33.47</v>
-      </c>
-      <c r="N26">
-        <v>0</v>
       </c>
       <c r="O26">
         <v>33.47</v>
       </c>
       <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>33.47</v>
+      </c>
+      <c r="R26">
         <v>28.16</v>
       </c>
-      <c r="Q26">
+      <c r="S26">
         <v>1616.64</v>
-      </c>
-      <c r="R26">
-        <v>0.17</v>
-      </c>
-      <c r="S26">
-        <v>0.17</v>
       </c>
       <c r="T26">
         <v>0.17</v>
@@ -5445,64 +5526,70 @@
       <c r="U26">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="27" spans="1:21">
+      <c r="V26">
+        <v>0.17</v>
+      </c>
+      <c r="W26">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
       <c r="A27" t="s">
-        <v>108</v>
-      </c>
-      <c r="B27">
+        <v>91</v>
+      </c>
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" t="s">
+        <v>102</v>
+      </c>
+      <c r="D27">
         <v>91.59999999999999</v>
       </c>
-      <c r="C27">
+      <c r="E27">
         <v>91.59999999999999</v>
       </c>
-      <c r="D27">
+      <c r="F27">
         <v>35.2</v>
       </c>
-      <c r="E27">
+      <c r="G27">
         <v>4.34</v>
       </c>
-      <c r="F27">
+      <c r="H27">
         <v>26.44</v>
       </c>
-      <c r="G27">
+      <c r="I27">
         <v>25.62</v>
       </c>
-      <c r="H27">
+      <c r="J27">
         <v>5.19</v>
       </c>
-      <c r="I27">
+      <c r="K27">
         <v>30.81</v>
       </c>
-      <c r="J27">
+      <c r="L27">
         <v>11.09</v>
       </c>
-      <c r="K27">
+      <c r="M27">
         <v>19.72</v>
       </c>
-      <c r="L27">
+      <c r="N27">
         <v>10.28</v>
-      </c>
-      <c r="M27">
-        <v>30</v>
-      </c>
-      <c r="N27">
-        <v>0</v>
       </c>
       <c r="O27">
         <v>30</v>
       </c>
       <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
         <v>30</v>
       </c>
-      <c r="Q27">
+      <c r="R27">
+        <v>30</v>
+      </c>
+      <c r="S27">
         <v>1616.64</v>
-      </c>
-      <c r="R27">
-        <v>0.19</v>
-      </c>
-      <c r="S27">
-        <v>0.22</v>
       </c>
       <c r="T27">
         <v>0.19</v>
@@ -5510,64 +5597,70 @@
       <c r="U27">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="28" spans="1:21">
+      <c r="V27">
+        <v>0.19</v>
+      </c>
+      <c r="W27">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
       <c r="A28" t="s">
-        <v>109</v>
-      </c>
-      <c r="B28">
+        <v>92</v>
+      </c>
+      <c r="B28" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28">
         <v>91.48</v>
       </c>
-      <c r="C28">
+      <c r="E28">
         <v>91.48</v>
       </c>
-      <c r="D28">
+      <c r="F28">
         <v>28.21</v>
       </c>
-      <c r="E28">
+      <c r="G28">
         <v>4.01</v>
       </c>
-      <c r="F28">
+      <c r="H28">
         <v>-26.51</v>
       </c>
-      <c r="G28">
+      <c r="I28">
         <v>85.77</v>
       </c>
-      <c r="H28">
+      <c r="J28">
         <v>2.12</v>
       </c>
-      <c r="I28">
+      <c r="K28">
         <v>87.89</v>
       </c>
-      <c r="J28">
+      <c r="L28">
         <v>10.65</v>
       </c>
-      <c r="K28">
+      <c r="M28">
         <v>77.23999999999999</v>
       </c>
-      <c r="L28">
+      <c r="N28">
         <v>-5.41</v>
       </c>
-      <c r="M28">
+      <c r="O28">
         <v>71.83</v>
       </c>
-      <c r="N28">
+      <c r="P28">
         <v>0.07000000000000001</v>
       </c>
-      <c r="O28">
+      <c r="Q28">
         <v>71.76000000000001</v>
       </c>
-      <c r="P28">
+      <c r="R28">
         <v>71.76000000000001</v>
       </c>
-      <c r="Q28">
+      <c r="S28">
         <v>1616.65</v>
-      </c>
-      <c r="R28">
-        <v>0.48</v>
-      </c>
-      <c r="S28">
-        <v>0.48</v>
       </c>
       <c r="T28">
         <v>0.48</v>
@@ -5575,64 +5668,70 @@
       <c r="U28">
         <v>0.48</v>
       </c>
-    </row>
-    <row r="29" spans="1:21">
+      <c r="V28">
+        <v>0.48</v>
+      </c>
+      <c r="W28">
+        <v>0.48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23">
       <c r="A29" t="s">
-        <v>110</v>
-      </c>
-      <c r="B29">
+        <v>92</v>
+      </c>
+      <c r="B29" t="s">
+        <v>100</v>
+      </c>
+      <c r="C29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D29">
         <v>81.58</v>
       </c>
-      <c r="C29">
+      <c r="E29">
         <v>81.58</v>
       </c>
-      <c r="D29">
+      <c r="F29">
         <v>34.9</v>
       </c>
-      <c r="E29">
+      <c r="G29">
         <v>4.16</v>
       </c>
-      <c r="F29">
+      <c r="H29">
         <v>7.97</v>
       </c>
-      <c r="G29">
+      <c r="I29">
         <v>34.55</v>
       </c>
-      <c r="H29">
+      <c r="J29">
         <v>5.01</v>
       </c>
-      <c r="I29">
+      <c r="K29">
         <v>39.56</v>
       </c>
-      <c r="J29">
+      <c r="L29">
         <v>9.710000000000001</v>
       </c>
-      <c r="K29">
+      <c r="M29">
         <v>29.85</v>
       </c>
-      <c r="L29">
+      <c r="N29">
         <v>-5.75</v>
       </c>
-      <c r="M29">
+      <c r="O29">
         <v>24.1</v>
       </c>
-      <c r="N29">
+      <c r="P29">
         <v>0.06</v>
       </c>
-      <c r="O29">
+      <c r="Q29">
         <v>24.04</v>
       </c>
-      <c r="P29">
+      <c r="R29">
         <v>24.04</v>
       </c>
-      <c r="Q29">
+      <c r="S29">
         <v>1616.65</v>
-      </c>
-      <c r="R29">
-        <v>0.18</v>
-      </c>
-      <c r="S29">
-        <v>0.18</v>
       </c>
       <c r="T29">
         <v>0.18</v>
@@ -5640,64 +5739,70 @@
       <c r="U29">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="30" spans="1:21">
+      <c r="V29">
+        <v>0.18</v>
+      </c>
+      <c r="W29">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
       <c r="A30" t="s">
-        <v>111</v>
-      </c>
-      <c r="B30">
+        <v>92</v>
+      </c>
+      <c r="B30" t="s">
+        <v>97</v>
+      </c>
+      <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30">
         <v>86.33</v>
       </c>
-      <c r="C30">
+      <c r="E30">
         <v>86.33</v>
       </c>
-      <c r="D30">
+      <c r="F30">
         <v>29.24</v>
       </c>
-      <c r="E30">
+      <c r="G30">
         <v>4.35</v>
       </c>
-      <c r="F30">
+      <c r="H30">
         <v>37.57</v>
       </c>
-      <c r="G30">
+      <c r="I30">
         <v>15.17</v>
       </c>
-      <c r="H30">
+      <c r="J30">
         <v>3.24</v>
       </c>
-      <c r="I30">
+      <c r="K30">
         <v>18.41</v>
       </c>
-      <c r="J30">
+      <c r="L30">
         <v>9.970000000000001</v>
       </c>
-      <c r="K30">
+      <c r="M30">
         <v>8.44</v>
       </c>
-      <c r="L30">
+      <c r="N30">
         <v>-5.67</v>
       </c>
-      <c r="M30">
+      <c r="O30">
         <v>2.77</v>
       </c>
-      <c r="N30">
+      <c r="P30">
         <v>0.19</v>
       </c>
-      <c r="O30">
+      <c r="Q30">
         <v>2.58</v>
       </c>
-      <c r="P30">
+      <c r="R30">
         <v>2.58</v>
       </c>
-      <c r="Q30">
+      <c r="S30">
         <v>1616.65</v>
-      </c>
-      <c r="R30">
-        <v>0.05</v>
-      </c>
-      <c r="S30">
-        <v>0.05</v>
       </c>
       <c r="T30">
         <v>0.05</v>
@@ -5705,64 +5810,70 @@
       <c r="U30">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="31" spans="1:21">
+      <c r="V30">
+        <v>0.05</v>
+      </c>
+      <c r="W30">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23">
       <c r="A31" t="s">
-        <v>112</v>
-      </c>
-      <c r="B31">
+        <v>92</v>
+      </c>
+      <c r="B31" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D31">
         <v>86.72</v>
       </c>
-      <c r="C31">
+      <c r="E31">
         <v>86.72</v>
       </c>
-      <c r="D31">
+      <c r="F31">
         <v>28.92</v>
       </c>
-      <c r="E31">
+      <c r="G31">
         <v>4.33</v>
       </c>
-      <c r="F31">
+      <c r="H31">
         <v>18.85</v>
       </c>
-      <c r="G31">
+      <c r="I31">
         <v>34.62</v>
       </c>
-      <c r="H31">
+      <c r="J31">
         <v>2.72</v>
       </c>
-      <c r="I31">
+      <c r="K31">
         <v>37.34</v>
       </c>
-      <c r="J31">
+      <c r="L31">
         <v>9.42</v>
       </c>
-      <c r="K31">
+      <c r="M31">
         <v>27.92</v>
       </c>
-      <c r="L31">
+      <c r="N31">
         <v>-8.15</v>
       </c>
-      <c r="M31">
+      <c r="O31">
         <v>19.77</v>
       </c>
-      <c r="N31">
+      <c r="P31">
         <v>-0.12</v>
       </c>
-      <c r="O31">
+      <c r="Q31">
         <v>19.89</v>
       </c>
-      <c r="P31">
+      <c r="R31">
         <v>19.89</v>
       </c>
-      <c r="Q31">
+      <c r="S31">
         <v>1616.65</v>
-      </c>
-      <c r="R31">
-        <v>0.16</v>
-      </c>
-      <c r="S31">
-        <v>0.16</v>
       </c>
       <c r="T31">
         <v>0.16</v>
@@ -5770,64 +5881,70 @@
       <c r="U31">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="32" spans="1:21">
+      <c r="V31">
+        <v>0.16</v>
+      </c>
+      <c r="W31">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23">
       <c r="A32" t="s">
-        <v>113</v>
-      </c>
-      <c r="B32">
+        <v>93</v>
+      </c>
+      <c r="B32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32">
         <v>52.22</v>
       </c>
-      <c r="C32">
+      <c r="E32">
         <v>52.22</v>
       </c>
-      <c r="D32">
+      <c r="F32">
         <v>37.42</v>
       </c>
-      <c r="E32">
+      <c r="G32">
         <v>2.63</v>
       </c>
-      <c r="F32">
+      <c r="H32">
         <v>48.8</v>
       </c>
-      <c r="G32">
+      <c r="I32">
         <v>-36.63</v>
       </c>
-      <c r="H32">
+      <c r="J32">
         <v>9.130000000000001</v>
       </c>
-      <c r="I32">
+      <c r="K32">
         <v>-27.5</v>
       </c>
-      <c r="J32">
+      <c r="L32">
         <v>8.35</v>
       </c>
-      <c r="K32">
+      <c r="M32">
         <v>-35.85</v>
       </c>
-      <c r="L32">
+      <c r="N32">
         <v>290.51</v>
       </c>
-      <c r="M32">
+      <c r="O32">
         <v>254.66</v>
       </c>
-      <c r="N32">
+      <c r="P32">
         <v>0.01</v>
       </c>
-      <c r="O32">
+      <c r="Q32">
         <v>254.65</v>
       </c>
-      <c r="P32">
+      <c r="R32">
         <v>277.91</v>
       </c>
-      <c r="Q32">
+      <c r="S32">
         <v>1616.65</v>
-      </c>
-      <c r="R32">
-        <v>1.61</v>
-      </c>
-      <c r="S32">
-        <v>1.61</v>
       </c>
       <c r="T32">
         <v>1.61</v>
@@ -5835,64 +5952,70 @@
       <c r="U32">
         <v>1.61</v>
       </c>
-    </row>
-    <row r="33" spans="1:21">
+      <c r="V32">
+        <v>1.61</v>
+      </c>
+      <c r="W32">
+        <v>1.61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23">
       <c r="A33" t="s">
-        <v>114</v>
-      </c>
-      <c r="B33">
+        <v>93</v>
+      </c>
+      <c r="B33" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" t="s">
+        <v>104</v>
+      </c>
+      <c r="D33">
         <v>53.1</v>
       </c>
-      <c r="C33">
+      <c r="E33">
         <v>53.1</v>
       </c>
-      <c r="D33">
+      <c r="F33">
         <v>22.69</v>
       </c>
-      <c r="E33">
+      <c r="G33">
         <v>2.45</v>
       </c>
-      <c r="F33">
+      <c r="H33">
         <v>22.11</v>
       </c>
-      <c r="G33">
+      <c r="I33">
         <v>5.85</v>
       </c>
-      <c r="H33">
+      <c r="J33">
         <v>3.73</v>
       </c>
-      <c r="I33">
+      <c r="K33">
         <v>9.58</v>
       </c>
-      <c r="J33">
+      <c r="L33">
         <v>1.93</v>
       </c>
-      <c r="K33">
+      <c r="M33">
         <v>7.65</v>
       </c>
-      <c r="L33">
+      <c r="N33">
         <v>14.1</v>
-      </c>
-      <c r="M33">
-        <v>21.75</v>
-      </c>
-      <c r="N33">
-        <v>0</v>
       </c>
       <c r="O33">
         <v>21.75</v>
       </c>
       <c r="P33">
+        <v>0</v>
+      </c>
+      <c r="Q33">
         <v>21.75</v>
       </c>
-      <c r="Q33">
+      <c r="R33">
+        <v>21.75</v>
+      </c>
+      <c r="S33">
         <v>1616.65</v>
-      </c>
-      <c r="R33">
-        <v>0.11</v>
-      </c>
-      <c r="S33">
-        <v>0.11</v>
       </c>
       <c r="T33">
         <v>0.11</v>
@@ -5900,64 +6023,70 @@
       <c r="U33">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="34" spans="1:21">
+      <c r="V33">
+        <v>0.11</v>
+      </c>
+      <c r="W33">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23">
       <c r="A34" t="s">
-        <v>115</v>
-      </c>
-      <c r="B34">
+        <v>93</v>
+      </c>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" t="s">
+        <v>101</v>
+      </c>
+      <c r="D34">
         <v>58.63</v>
       </c>
-      <c r="C34">
+      <c r="E34">
         <v>58.63</v>
       </c>
-      <c r="D34">
+      <c r="F34">
         <v>28.07</v>
       </c>
-      <c r="E34">
+      <c r="G34">
         <v>2.68</v>
       </c>
-      <c r="F34">
+      <c r="H34">
         <v>46.09</v>
       </c>
-      <c r="G34">
+      <c r="I34">
         <v>-18.21</v>
       </c>
-      <c r="H34">
+      <c r="J34">
         <v>4.69</v>
       </c>
-      <c r="I34">
+      <c r="K34">
         <v>-13.52</v>
       </c>
-      <c r="J34">
+      <c r="L34">
         <v>2.15</v>
       </c>
-      <c r="K34">
+      <c r="M34">
         <v>-15.67</v>
       </c>
-      <c r="L34">
+      <c r="N34">
         <v>3.25</v>
-      </c>
-      <c r="M34">
-        <v>-12.42</v>
-      </c>
-      <c r="N34">
-        <v>0</v>
       </c>
       <c r="O34">
         <v>-12.42</v>
       </c>
       <c r="P34">
+        <v>0</v>
+      </c>
+      <c r="Q34">
         <v>-12.42</v>
       </c>
-      <c r="Q34">
+      <c r="R34">
+        <v>-12.42</v>
+      </c>
+      <c r="S34">
         <v>161.67</v>
-      </c>
-      <c r="R34">
-        <v>-0.77</v>
-      </c>
-      <c r="S34">
-        <v>-0.77</v>
       </c>
       <c r="T34">
         <v>-0.77</v>
@@ -5965,64 +6094,70 @@
       <c r="U34">
         <v>-0.77</v>
       </c>
-    </row>
-    <row r="35" spans="1:21">
+      <c r="V34">
+        <v>-0.77</v>
+      </c>
+      <c r="W34">
+        <v>-0.77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23">
       <c r="A35" t="s">
-        <v>116</v>
-      </c>
-      <c r="B35">
+        <v>93</v>
+      </c>
+      <c r="B35" t="s">
+        <v>98</v>
+      </c>
+      <c r="C35" t="s">
+        <v>102</v>
+      </c>
+      <c r="D35">
         <v>46.86</v>
       </c>
-      <c r="C35">
+      <c r="E35">
         <v>46.86</v>
       </c>
-      <c r="D35">
+      <c r="F35">
         <v>30.42</v>
       </c>
-      <c r="E35">
+      <c r="G35">
         <v>3.16</v>
       </c>
-      <c r="F35">
+      <c r="H35">
         <v>27.48</v>
       </c>
-      <c r="G35">
+      <c r="I35">
         <v>-14.2</v>
       </c>
-      <c r="H35">
+      <c r="J35">
         <v>3.27</v>
       </c>
-      <c r="I35">
+      <c r="K35">
         <v>-10.93</v>
       </c>
-      <c r="J35">
+      <c r="L35">
         <v>2.23</v>
       </c>
-      <c r="K35">
+      <c r="M35">
         <v>-13.16</v>
       </c>
-      <c r="L35">
+      <c r="N35">
         <v>-8.609999999999999</v>
-      </c>
-      <c r="M35">
-        <v>-21.77</v>
-      </c>
-      <c r="N35">
-        <v>0</v>
       </c>
       <c r="O35">
         <v>-21.77</v>
       </c>
       <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
         <v>-21.77</v>
       </c>
-      <c r="Q35">
+      <c r="R35">
+        <v>-21.77</v>
+      </c>
+      <c r="S35">
         <v>165.44</v>
-      </c>
-      <c r="R35">
-        <v>-1.32</v>
-      </c>
-      <c r="S35">
-        <v>-1.32</v>
       </c>
       <c r="T35">
         <v>-1.32</v>
@@ -6030,64 +6165,70 @@
       <c r="U35">
         <v>-1.32</v>
       </c>
-    </row>
-    <row r="36" spans="1:21">
+      <c r="V35">
+        <v>-1.32</v>
+      </c>
+      <c r="W35">
+        <v>-1.32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23">
       <c r="A36" t="s">
-        <v>117</v>
-      </c>
-      <c r="B36">
+        <v>94</v>
+      </c>
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36">
         <v>54.01</v>
       </c>
-      <c r="C36">
+      <c r="E36">
         <v>54.01</v>
       </c>
-      <c r="D36">
+      <c r="F36">
         <v>24.11</v>
       </c>
-      <c r="E36">
+      <c r="G36">
         <v>4.4</v>
       </c>
-      <c r="F36">
+      <c r="H36">
         <v>20.72</v>
       </c>
-      <c r="G36">
+      <c r="I36">
         <v>4.78</v>
       </c>
-      <c r="H36">
+      <c r="J36">
         <v>1.6</v>
       </c>
-      <c r="I36">
+      <c r="K36">
         <v>6.38</v>
       </c>
-      <c r="J36">
+      <c r="L36">
         <v>2.45</v>
       </c>
-      <c r="K36">
+      <c r="M36">
         <v>3.93</v>
       </c>
-      <c r="L36">
+      <c r="N36">
         <v>16.93</v>
-      </c>
-      <c r="M36">
-        <v>20.86</v>
-      </c>
-      <c r="N36">
-        <v>0</v>
       </c>
       <c r="O36">
         <v>20.86</v>
       </c>
       <c r="P36">
+        <v>0</v>
+      </c>
+      <c r="Q36">
         <v>20.86</v>
       </c>
-      <c r="Q36">
+      <c r="R36">
+        <v>20.86</v>
+      </c>
+      <c r="S36">
         <v>167.94</v>
-      </c>
-      <c r="R36">
-        <v>1.25</v>
-      </c>
-      <c r="S36">
-        <v>1.25</v>
       </c>
       <c r="T36">
         <v>1.25</v>
@@ -6095,43 +6236,49 @@
       <c r="U36">
         <v>1.25</v>
       </c>
-    </row>
-    <row r="37" spans="1:21">
+      <c r="V36">
+        <v>1.25</v>
+      </c>
+      <c r="W36">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
       <c r="A37" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37">
+        <v>94</v>
+      </c>
+      <c r="B37" t="s">
+        <v>100</v>
+      </c>
+      <c r="C37" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37">
         <v>62.58</v>
       </c>
-      <c r="C37">
+      <c r="E37">
         <v>62.58</v>
       </c>
-      <c r="D37">
+      <c r="F37">
         <v>32.91</v>
       </c>
-      <c r="E37">
+      <c r="G37">
         <v>4.49</v>
       </c>
-      <c r="F37">
+      <c r="H37">
         <v>4.88</v>
       </c>
-      <c r="G37">
+      <c r="I37">
         <v>20.3</v>
       </c>
-      <c r="H37">
+      <c r="J37">
         <v>3.39</v>
       </c>
-      <c r="I37">
+      <c r="K37">
         <v>23.69</v>
       </c>
-      <c r="J37">
+      <c r="L37">
         <v>-1.85</v>
-      </c>
-      <c r="K37">
-        <v>25.54</v>
-      </c>
-      <c r="L37">
-        <v>0</v>
       </c>
       <c r="M37">
         <v>25.54</v>
@@ -6143,16 +6290,16 @@
         <v>25.54</v>
       </c>
       <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
         <v>25.54</v>
       </c>
-      <c r="Q37">
+      <c r="R37">
+        <v>25.54</v>
+      </c>
+      <c r="S37">
         <v>168.38</v>
-      </c>
-      <c r="R37">
-        <v>1.52</v>
-      </c>
-      <c r="S37">
-        <v>1.52</v>
       </c>
       <c r="T37">
         <v>1.52</v>
@@ -6160,64 +6307,70 @@
       <c r="U37">
         <v>1.52</v>
       </c>
-    </row>
-    <row r="38" spans="1:21">
+      <c r="V37">
+        <v>1.52</v>
+      </c>
+      <c r="W37">
+        <v>1.52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23">
       <c r="A38" t="s">
-        <v>119</v>
-      </c>
-      <c r="B38">
+        <v>94</v>
+      </c>
+      <c r="B38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" t="s">
+        <v>101</v>
+      </c>
+      <c r="D38">
         <v>68.62</v>
       </c>
-      <c r="C38">
+      <c r="E38">
         <v>68.62</v>
       </c>
-      <c r="D38">
+      <c r="F38">
         <v>42.39</v>
       </c>
-      <c r="E38">
+      <c r="G38">
         <v>4.5</v>
       </c>
-      <c r="F38">
+      <c r="H38">
         <v>7.04</v>
       </c>
-      <c r="G38">
+      <c r="I38">
         <v>14.69</v>
       </c>
-      <c r="H38">
+      <c r="J38">
         <v>2.19</v>
       </c>
-      <c r="I38">
+      <c r="K38">
         <v>16.88</v>
       </c>
-      <c r="J38">
+      <c r="L38">
         <v>2.36</v>
       </c>
-      <c r="K38">
+      <c r="M38">
         <v>14.52</v>
       </c>
-      <c r="L38">
+      <c r="N38">
         <v>-7.75</v>
-      </c>
-      <c r="M38">
-        <v>6.77</v>
-      </c>
-      <c r="N38">
-        <v>0</v>
       </c>
       <c r="O38">
         <v>6.77</v>
       </c>
       <c r="P38">
+        <v>0</v>
+      </c>
+      <c r="Q38">
         <v>6.77</v>
       </c>
-      <c r="Q38">
+      <c r="R38">
+        <v>6.77</v>
+      </c>
+      <c r="S38">
         <v>168.39</v>
-      </c>
-      <c r="R38">
-        <v>0.4</v>
-      </c>
-      <c r="S38">
-        <v>0.05</v>
       </c>
       <c r="T38">
         <v>0.4</v>
@@ -6225,64 +6378,70 @@
       <c r="U38">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="39" spans="1:21">
+      <c r="V38">
+        <v>0.4</v>
+      </c>
+      <c r="W38">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23">
       <c r="A39" t="s">
-        <v>120</v>
-      </c>
-      <c r="B39">
+        <v>94</v>
+      </c>
+      <c r="B39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" t="s">
+        <v>102</v>
+      </c>
+      <c r="D39">
         <v>69.65000000000001</v>
       </c>
-      <c r="C39">
+      <c r="E39">
         <v>69.65000000000001</v>
       </c>
-      <c r="D39">
+      <c r="F39">
         <v>36.91</v>
       </c>
-      <c r="E39">
+      <c r="G39">
         <v>7.18</v>
       </c>
-      <c r="F39">
+      <c r="H39">
         <v>4.22</v>
       </c>
-      <c r="G39">
+      <c r="I39">
         <v>21.34</v>
       </c>
-      <c r="H39">
+      <c r="J39">
         <v>3.56</v>
       </c>
-      <c r="I39">
+      <c r="K39">
         <v>24.9</v>
       </c>
-      <c r="J39">
+      <c r="L39">
         <v>6.49</v>
       </c>
-      <c r="K39">
+      <c r="M39">
         <v>18.41</v>
       </c>
-      <c r="L39">
+      <c r="N39">
         <v>23.09</v>
-      </c>
-      <c r="M39">
-        <v>41.5</v>
-      </c>
-      <c r="N39">
-        <v>0</v>
       </c>
       <c r="O39">
         <v>41.5</v>
       </c>
       <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="Q39">
         <v>41.5</v>
       </c>
-      <c r="Q39">
+      <c r="R39">
+        <v>41.5</v>
+      </c>
+      <c r="S39">
         <v>168.39</v>
-      </c>
-      <c r="R39">
-        <v>2.46</v>
-      </c>
-      <c r="S39">
-        <v>0</v>
       </c>
       <c r="T39">
         <v>2.46</v>
@@ -6290,64 +6449,70 @@
       <c r="U39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:21">
+      <c r="V39">
+        <v>2.46</v>
+      </c>
+      <c r="W39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23">
       <c r="A40" t="s">
-        <v>121</v>
-      </c>
-      <c r="B40">
+        <v>95</v>
+      </c>
+      <c r="B40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" t="s">
+        <v>103</v>
+      </c>
+      <c r="D40">
         <v>75.40000000000001</v>
       </c>
-      <c r="C40">
+      <c r="E40">
         <v>75.40000000000001</v>
       </c>
-      <c r="D40">
+      <c r="F40">
         <v>36.16</v>
       </c>
-      <c r="E40">
+      <c r="G40">
         <v>5.03</v>
       </c>
-      <c r="F40">
+      <c r="H40">
         <v>56.15</v>
       </c>
-      <c r="G40">
+      <c r="I40">
         <v>-21.94</v>
       </c>
-      <c r="H40">
+      <c r="J40">
         <v>3.24</v>
       </c>
-      <c r="I40">
+      <c r="K40">
         <v>-18.7</v>
       </c>
-      <c r="J40">
+      <c r="L40">
         <v>2</v>
       </c>
-      <c r="K40">
+      <c r="M40">
         <v>-20.7</v>
       </c>
-      <c r="L40">
+      <c r="N40">
         <v>-0.86</v>
-      </c>
-      <c r="M40">
-        <v>-21.56</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
       </c>
       <c r="O40">
         <v>-21.56</v>
       </c>
       <c r="P40">
+        <v>0</v>
+      </c>
+      <c r="Q40">
         <v>-21.56</v>
       </c>
-      <c r="Q40">
+      <c r="R40">
+        <v>-21.56</v>
+      </c>
+      <c r="S40">
         <v>168.47</v>
-      </c>
-      <c r="R40">
-        <v>-1.28</v>
-      </c>
-      <c r="S40">
-        <v>-1.28</v>
       </c>
       <c r="T40">
         <v>-1.28</v>
@@ -6355,64 +6520,70 @@
       <c r="U40">
         <v>-1.28</v>
       </c>
-    </row>
-    <row r="41" spans="1:21">
+      <c r="V40">
+        <v>-1.28</v>
+      </c>
+      <c r="W40">
+        <v>-1.28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23">
       <c r="A41" t="s">
-        <v>122</v>
-      </c>
-      <c r="B41">
+        <v>95</v>
+      </c>
+      <c r="B41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41">
         <v>82.78</v>
       </c>
-      <c r="C41">
+      <c r="E41">
         <v>82.78</v>
       </c>
-      <c r="D41">
+      <c r="F41">
         <v>37.48</v>
       </c>
-      <c r="E41">
+      <c r="G41">
         <v>5.02</v>
       </c>
-      <c r="F41">
+      <c r="H41">
         <v>51.41</v>
       </c>
-      <c r="G41">
+      <c r="I41">
         <v>-11.13</v>
       </c>
-      <c r="H41">
+      <c r="J41">
         <v>0.9</v>
       </c>
-      <c r="I41">
+      <c r="K41">
         <v>-10.23</v>
       </c>
-      <c r="J41">
+      <c r="L41">
         <v>2.17</v>
       </c>
-      <c r="K41">
+      <c r="M41">
         <v>-12.4</v>
       </c>
-      <c r="L41">
+      <c r="N41">
         <v>-2.9</v>
-      </c>
-      <c r="M41">
-        <v>-15.3</v>
-      </c>
-      <c r="N41">
-        <v>0</v>
       </c>
       <c r="O41">
         <v>-15.3</v>
       </c>
       <c r="P41">
+        <v>0</v>
+      </c>
+      <c r="Q41">
         <v>-15.3</v>
       </c>
-      <c r="Q41">
+      <c r="R41">
+        <v>-15.3</v>
+      </c>
+      <c r="S41">
         <v>168.47</v>
-      </c>
-      <c r="R41">
-        <v>-0.91</v>
-      </c>
-      <c r="S41">
-        <v>-0.91</v>
       </c>
       <c r="T41">
         <v>-0.91</v>
@@ -6420,43 +6591,49 @@
       <c r="U41">
         <v>-0.91</v>
       </c>
-    </row>
-    <row r="42" spans="1:21">
+      <c r="V41">
+        <v>-0.91</v>
+      </c>
+      <c r="W41">
+        <v>-0.91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23">
       <c r="A42" t="s">
-        <v>123</v>
-      </c>
-      <c r="B42">
+        <v>95</v>
+      </c>
+      <c r="B42" t="s">
+        <v>97</v>
+      </c>
+      <c r="C42" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42">
         <v>91.06999999999999</v>
       </c>
-      <c r="C42">
+      <c r="E42">
         <v>91.06999999999999</v>
       </c>
-      <c r="D42">
+      <c r="F42">
         <v>46.58</v>
       </c>
-      <c r="E42">
+      <c r="G42">
         <v>6.52</v>
       </c>
-      <c r="F42">
+      <c r="H42">
         <v>152.21</v>
       </c>
-      <c r="G42">
+      <c r="I42">
         <v>-114.24</v>
       </c>
-      <c r="H42">
+      <c r="J42">
         <v>1.68</v>
       </c>
-      <c r="I42">
+      <c r="K42">
         <v>-112.56</v>
       </c>
-      <c r="J42">
+      <c r="L42">
         <v>2.22</v>
-      </c>
-      <c r="K42">
-        <v>-114.78</v>
-      </c>
-      <c r="L42">
-        <v>0</v>
       </c>
       <c r="M42">
         <v>-114.78</v>
@@ -6468,16 +6645,16 @@
         <v>-114.78</v>
       </c>
       <c r="P42">
+        <v>0</v>
+      </c>
+      <c r="Q42">
         <v>-114.78</v>
       </c>
-      <c r="Q42">
+      <c r="R42">
+        <v>-114.78</v>
+      </c>
+      <c r="S42">
         <v>168.64</v>
-      </c>
-      <c r="R42">
-        <v>-6.81</v>
-      </c>
-      <c r="S42">
-        <v>-6.78</v>
       </c>
       <c r="T42">
         <v>-6.81</v>
@@ -6485,64 +6662,70 @@
       <c r="U42">
         <v>-6.78</v>
       </c>
-    </row>
-    <row r="43" spans="1:21">
+      <c r="V42">
+        <v>-6.81</v>
+      </c>
+      <c r="W42">
+        <v>-6.78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23">
       <c r="A43" t="s">
-        <v>124</v>
-      </c>
-      <c r="B43">
+        <v>95</v>
+      </c>
+      <c r="B43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" t="s">
+        <v>102</v>
+      </c>
+      <c r="D43">
         <v>91.64</v>
       </c>
-      <c r="C43">
+      <c r="E43">
         <v>91.64</v>
       </c>
-      <c r="D43">
+      <c r="F43">
         <v>48.66</v>
       </c>
-      <c r="E43">
+      <c r="G43">
         <v>6.29</v>
       </c>
-      <c r="F43">
+      <c r="H43">
         <v>257.95</v>
       </c>
-      <c r="G43">
+      <c r="I43">
         <v>-221.26</v>
       </c>
-      <c r="H43">
+      <c r="J43">
         <v>2.34</v>
       </c>
-      <c r="I43">
+      <c r="K43">
         <v>-218.92</v>
       </c>
-      <c r="J43">
+      <c r="L43">
         <v>2.29</v>
       </c>
-      <c r="K43">
+      <c r="M43">
         <v>-221.21</v>
       </c>
-      <c r="L43">
+      <c r="N43">
         <v>-421.7</v>
-      </c>
-      <c r="M43">
-        <v>-642.91</v>
-      </c>
-      <c r="N43">
-        <v>0</v>
       </c>
       <c r="O43">
         <v>-642.91</v>
       </c>
       <c r="P43">
+        <v>0</v>
+      </c>
+      <c r="Q43">
         <v>-642.91</v>
       </c>
-      <c r="Q43">
+      <c r="R43">
+        <v>-642.91</v>
+      </c>
+      <c r="S43">
         <v>168.77</v>
-      </c>
-      <c r="R43">
-        <v>-38.1</v>
-      </c>
-      <c r="S43">
-        <v>-38.1</v>
       </c>
       <c r="T43">
         <v>-38.1</v>
@@ -6550,64 +6733,70 @@
       <c r="U43">
         <v>-38.1</v>
       </c>
-    </row>
-    <row r="44" spans="1:21">
+      <c r="V43">
+        <v>-38.1</v>
+      </c>
+      <c r="W43">
+        <v>-38.1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23">
       <c r="A44" t="s">
-        <v>125</v>
-      </c>
-      <c r="B44">
+        <v>96</v>
+      </c>
+      <c r="B44" t="s">
+        <v>99</v>
+      </c>
+      <c r="C44" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44">
         <v>91.83</v>
       </c>
-      <c r="C44">
+      <c r="E44">
         <v>91.83</v>
       </c>
-      <c r="D44">
+      <c r="F44">
         <v>52.08</v>
       </c>
-      <c r="E44">
+      <c r="G44">
         <v>6.98</v>
       </c>
-      <c r="F44">
+      <c r="H44">
         <v>84.15000000000001</v>
       </c>
-      <c r="G44">
+      <c r="I44">
         <v>-51.38</v>
       </c>
-      <c r="H44">
+      <c r="J44">
         <v>3.55</v>
       </c>
-      <c r="I44">
+      <c r="K44">
         <v>-47.83</v>
       </c>
-      <c r="J44">
+      <c r="L44">
         <v>2.04</v>
       </c>
-      <c r="K44">
+      <c r="M44">
         <v>-49.87</v>
       </c>
-      <c r="L44">
+      <c r="N44">
         <v>4.23</v>
-      </c>
-      <c r="M44">
-        <v>-45.64</v>
-      </c>
-      <c r="N44">
-        <v>0</v>
       </c>
       <c r="O44">
         <v>-45.64</v>
       </c>
       <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
         <v>-45.64</v>
       </c>
-      <c r="Q44">
+      <c r="R44">
+        <v>-45.64</v>
+      </c>
+      <c r="S44">
         <v>169.23</v>
-      </c>
-      <c r="R44">
-        <v>-2.7</v>
-      </c>
-      <c r="S44">
-        <v>-2.7</v>
       </c>
       <c r="T44">
         <v>-2.7</v>
@@ -6615,43 +6804,49 @@
       <c r="U44">
         <v>-2.7</v>
       </c>
-    </row>
-    <row r="45" spans="1:21">
+      <c r="V44">
+        <v>-2.7</v>
+      </c>
+      <c r="W44">
+        <v>-2.7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23">
       <c r="A45" t="s">
-        <v>126</v>
-      </c>
-      <c r="B45">
+        <v>96</v>
+      </c>
+      <c r="B45" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" t="s">
+        <v>104</v>
+      </c>
+      <c r="D45">
         <v>89.77</v>
       </c>
-      <c r="C45">
+      <c r="E45">
         <v>89.77</v>
       </c>
-      <c r="D45">
+      <c r="F45">
         <v>52.28</v>
       </c>
-      <c r="E45">
+      <c r="G45">
         <v>6.11</v>
       </c>
-      <c r="F45">
+      <c r="H45">
         <v>40.06</v>
       </c>
-      <c r="G45">
+      <c r="I45">
         <v>-8.68</v>
       </c>
-      <c r="H45">
+      <c r="J45">
         <v>1.62</v>
       </c>
-      <c r="I45">
+      <c r="K45">
         <v>-7.06</v>
       </c>
-      <c r="J45">
+      <c r="L45">
         <v>1.94</v>
-      </c>
-      <c r="K45">
-        <v>-9</v>
-      </c>
-      <c r="L45">
-        <v>0</v>
       </c>
       <c r="M45">
         <v>-9</v>
@@ -6663,16 +6858,16 @@
         <v>-9</v>
       </c>
       <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
         <v>-9</v>
       </c>
-      <c r="Q45">
+      <c r="R45">
+        <v>-9</v>
+      </c>
+      <c r="S45">
         <v>169.24</v>
-      </c>
-      <c r="R45">
-        <v>-0.53</v>
-      </c>
-      <c r="S45">
-        <v>-0.53</v>
       </c>
       <c r="T45">
         <v>-0.53</v>
@@ -6680,43 +6875,49 @@
       <c r="U45">
         <v>-0.53</v>
       </c>
-    </row>
-    <row r="46" spans="1:21">
+      <c r="V45">
+        <v>-0.53</v>
+      </c>
+      <c r="W45">
+        <v>-0.53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23">
       <c r="A46" t="s">
-        <v>127</v>
-      </c>
-      <c r="B46">
+        <v>96</v>
+      </c>
+      <c r="B46" t="s">
+        <v>97</v>
+      </c>
+      <c r="C46" t="s">
+        <v>101</v>
+      </c>
+      <c r="D46">
         <v>89.40000000000001</v>
       </c>
-      <c r="C46">
+      <c r="E46">
         <v>89.40000000000001</v>
       </c>
-      <c r="D46">
+      <c r="F46">
         <v>50.49</v>
       </c>
-      <c r="E46">
+      <c r="G46">
         <v>6.46</v>
       </c>
-      <c r="F46">
+      <c r="H46">
         <v>18.72</v>
       </c>
-      <c r="G46">
+      <c r="I46">
         <v>13.73</v>
       </c>
-      <c r="H46">
+      <c r="J46">
         <v>1.95</v>
       </c>
-      <c r="I46">
+      <c r="K46">
         <v>15.68</v>
       </c>
-      <c r="J46">
+      <c r="L46">
         <v>2.15</v>
-      </c>
-      <c r="K46">
-        <v>13.53</v>
-      </c>
-      <c r="L46">
-        <v>0</v>
       </c>
       <c r="M46">
         <v>13.53</v>
@@ -6728,21 +6929,27 @@
         <v>13.53</v>
       </c>
       <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
         <v>13.53</v>
       </c>
-      <c r="Q46">
+      <c r="R46">
+        <v>13.53</v>
+      </c>
+      <c r="S46">
         <v>169.4</v>
-      </c>
-      <c r="R46">
-        <v>0.8</v>
-      </c>
-      <c r="S46">
-        <v>0.79</v>
       </c>
       <c r="T46">
         <v>0.8</v>
       </c>
       <c r="U46">
+        <v>0.79</v>
+      </c>
+      <c r="V46">
+        <v>0.8</v>
+      </c>
+      <c r="W46">
         <v>0.79</v>
       </c>
     </row>
@@ -6761,58 +6968,58 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>129</v>
+        <v>106</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>130</v>
+        <v>107</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>133</v>
+        <v>110</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>134</v>
+        <v>111</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>135</v>
+        <v>112</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>136</v>
+        <v>113</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>137</v>
+        <v>114</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>138</v>
+        <v>115</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>139</v>
+        <v>116</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>140</v>
+        <v>117</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>143</v>
+        <v>120</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>144</v>
+        <v>121</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:18">

</xml_diff>